<commit_message>
update extreme case analysis
</commit_message>
<xml_diff>
--- a/Data/ExtremeCases.xlsx
+++ b/Data/ExtremeCases.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27080" yWindow="1880" windowWidth="25120" windowHeight="14300" tabRatio="500"/>
+    <workbookView xWindow="-31980" yWindow="-3840" windowWidth="25120" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Trees" sheetId="2" r:id="rId2"/>
+    <sheet name="Lightning" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -95,12 +97,15 @@
   <si>
     <t>rain, ahil, thunderstorm</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,6 +125,22 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -156,8 +177,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -187,7 +226,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -702,40 +759,40 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2">
-        <v>41580</v>
+        <v>42094</v>
       </c>
       <c r="B5" s="3">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G5">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J5">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="K5">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>0.04</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -743,40 +800,40 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2">
-        <v>42094</v>
+        <v>41580</v>
       </c>
       <c r="B6" s="3">
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H6">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I6">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J6">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="K6">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L6">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -1144,84 +1201,84 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2">
-        <v>42022</v>
+        <v>42230</v>
       </c>
       <c r="B16" s="3">
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G16">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="H16">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J16">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K16">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="L16">
-        <v>0.84</v>
+        <v>1.2</v>
       </c>
       <c r="M16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2">
-        <v>42230</v>
+        <v>42022</v>
       </c>
       <c r="B17" s="3">
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
         <v>0</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
       <c r="F17">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G17">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="H17">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I17">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J17">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="K17">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="L17">
-        <v>1.2</v>
+        <v>0.84</v>
       </c>
       <c r="M17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1589,13 +1646,13 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2">
-        <v>41972</v>
+        <v>42228</v>
       </c>
       <c r="B27" s="3">
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1604,42 +1661,39 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="G27">
+        <v>56</v>
+      </c>
+      <c r="H27">
+        <v>59</v>
+      </c>
+      <c r="I27">
+        <v>6</v>
+      </c>
+      <c r="J27">
+        <v>17</v>
+      </c>
+      <c r="K27">
+        <v>22</v>
+      </c>
+      <c r="L27">
+        <v>0.3</v>
+      </c>
+      <c r="M27" t="s">
         <v>24</v>
-      </c>
-      <c r="H27">
-        <v>71</v>
-      </c>
-      <c r="I27">
-        <v>12</v>
-      </c>
-      <c r="J27">
-        <v>31</v>
-      </c>
-      <c r="K27">
-        <v>39</v>
-      </c>
-      <c r="L27">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M27" t="s">
-        <v>20</v>
-      </c>
-      <c r="N27">
-        <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="2">
-        <v>42228</v>
+        <v>41972</v>
       </c>
       <c r="B28" s="3">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1648,28 +1702,31 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="G28">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="H28">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="I28">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J28">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="K28">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="L28">
-        <v>0.3</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M28" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="N28">
+        <v>0.8</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1797,81 +1854,57 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="2">
-        <v>37176</v>
+        <v>41446</v>
       </c>
       <c r="B32" s="3">
         <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
         <v>1</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>52</v>
-      </c>
-      <c r="G32">
-        <v>47</v>
-      </c>
-      <c r="H32">
-        <v>85</v>
-      </c>
-      <c r="I32">
-        <v>14</v>
-      </c>
-      <c r="J32">
-        <v>29</v>
-      </c>
-      <c r="K32">
-        <v>34</v>
-      </c>
-      <c r="L32">
-        <v>0.04</v>
-      </c>
-      <c r="M32" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2">
-        <v>40497</v>
+        <v>37176</v>
       </c>
       <c r="B33" s="3">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>52</v>
       </c>
       <c r="G33">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H33">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I33">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J33">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="K33">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="L33">
-        <v>0.14000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="M33" t="s">
         <v>18</v>
@@ -1879,53 +1912,77 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="2">
-        <v>41446</v>
+        <v>40497</v>
       </c>
       <c r="B34" s="3">
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
+      <c r="F34">
+        <v>52</v>
+      </c>
+      <c r="G34">
+        <v>49</v>
+      </c>
+      <c r="H34">
+        <v>82</v>
+      </c>
+      <c r="I34">
+        <v>15</v>
+      </c>
+      <c r="J34">
+        <v>36</v>
+      </c>
+      <c r="K34">
+        <v>49</v>
+      </c>
+      <c r="L34">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M34" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="2">
-        <v>37360</v>
+        <v>41451</v>
       </c>
       <c r="B35" s="3">
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
         <v>2</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="2">
-        <v>41451</v>
+        <v>37360</v>
       </c>
       <c r="B36" s="3">
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -1947,36 +2004,36 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="2">
-        <v>39608</v>
+        <v>39968</v>
       </c>
       <c r="B38" s="3">
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="2">
-        <v>39968</v>
+        <v>39608</v>
       </c>
       <c r="B39" s="3">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
         <v>0</v>
-      </c>
-      <c r="E39">
-        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2005,8 +2062,18 @@
       <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="2"/>
+      <c r="A43" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B43" s="3"/>
+      <c r="D43">
+        <f>AVERAGE(D2:D40)</f>
+        <v>2.1052631578947367</v>
+      </c>
+      <c r="E43">
+        <f>AVERAGE(E2:E40)</f>
+        <v>1.1578947368421053</v>
+      </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="2"/>
@@ -19703,6 +19770,1400 @@
     <row r="4467" spans="1:2">
       <c r="A4467" s="4"/>
       <c r="B4467" s="5"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:N4467">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2">
+        <v>42245</v>
+      </c>
+      <c r="B1" s="3">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>64</v>
+      </c>
+      <c r="G1">
+        <v>56</v>
+      </c>
+      <c r="H1">
+        <v>72</v>
+      </c>
+      <c r="I1">
+        <v>13</v>
+      </c>
+      <c r="J1">
+        <v>35</v>
+      </c>
+      <c r="K1">
+        <v>46</v>
+      </c>
+      <c r="L1">
+        <v>1.28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2">
+        <v>38752</v>
+      </c>
+      <c r="B2" s="3">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>48</v>
+      </c>
+      <c r="G2">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>75</v>
+      </c>
+      <c r="I2">
+        <v>21</v>
+      </c>
+      <c r="J2">
+        <v>36</v>
+      </c>
+      <c r="K2">
+        <v>47</v>
+      </c>
+      <c r="L2">
+        <v>0.41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2">
+        <v>41580</v>
+      </c>
+      <c r="B3" s="3">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>53</v>
+      </c>
+      <c r="G3">
+        <v>42</v>
+      </c>
+      <c r="H3">
+        <v>69</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>43</v>
+      </c>
+      <c r="K3">
+        <v>59</v>
+      </c>
+      <c r="L3">
+        <v>0.5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2">
+        <v>37993</v>
+      </c>
+      <c r="B4" s="3">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>90</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2">
+        <v>41937</v>
+      </c>
+      <c r="B5" s="3">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>55</v>
+      </c>
+      <c r="G5">
+        <v>49</v>
+      </c>
+      <c r="H5">
+        <v>81</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+      <c r="J5">
+        <v>37</v>
+      </c>
+      <c r="K5">
+        <v>49</v>
+      </c>
+      <c r="L5">
+        <v>0.24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2">
+        <v>39066</v>
+      </c>
+      <c r="B6" s="3">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>57</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <v>69</v>
+      </c>
+      <c r="L6">
+        <v>0.02</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2">
+        <v>39065</v>
+      </c>
+      <c r="B7" s="3">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>47</v>
+      </c>
+      <c r="G7">
+        <v>44</v>
+      </c>
+      <c r="H7">
+        <v>81</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>47</v>
+      </c>
+      <c r="K7">
+        <v>60</v>
+      </c>
+      <c r="L7">
+        <v>1.55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2">
+        <v>39373</v>
+      </c>
+      <c r="B8" s="3">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>53</v>
+      </c>
+      <c r="G8">
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <v>77</v>
+      </c>
+      <c r="I8">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <v>39</v>
+      </c>
+      <c r="K8">
+        <v>53</v>
+      </c>
+      <c r="L8">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2">
+        <v>36541</v>
+      </c>
+      <c r="B9" s="3">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>36</v>
+      </c>
+      <c r="H9">
+        <v>86</v>
+      </c>
+      <c r="I9">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>36</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2">
+        <v>42325</v>
+      </c>
+      <c r="B10" s="3">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>85</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>37</v>
+      </c>
+      <c r="K10">
+        <v>51</v>
+      </c>
+      <c r="L10">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2">
+        <v>42022</v>
+      </c>
+      <c r="B11" s="3">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>51</v>
+      </c>
+      <c r="G11">
+        <v>44</v>
+      </c>
+      <c r="H11">
+        <v>80</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>40</v>
+      </c>
+      <c r="K11">
+        <v>59</v>
+      </c>
+      <c r="L11">
+        <v>0.84</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2">
+        <v>42442</v>
+      </c>
+      <c r="B12" s="3">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>47</v>
+      </c>
+      <c r="G12">
+        <v>38</v>
+      </c>
+      <c r="H12">
+        <v>76</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
+      </c>
+      <c r="J12">
+        <v>44</v>
+      </c>
+      <c r="K12">
+        <v>57</v>
+      </c>
+      <c r="L12">
+        <v>0.62</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2">
+        <v>37959</v>
+      </c>
+      <c r="B13" s="3">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>44</v>
+      </c>
+      <c r="G13">
+        <v>31</v>
+      </c>
+      <c r="H13">
+        <v>61</v>
+      </c>
+      <c r="I13">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>29</v>
+      </c>
+      <c r="K13">
+        <v>45</v>
+      </c>
+      <c r="L13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="2">
+        <v>39725</v>
+      </c>
+      <c r="B14" s="3">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>56</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>79</v>
+      </c>
+      <c r="I14">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>28</v>
+      </c>
+      <c r="K14">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="2">
+        <v>41984</v>
+      </c>
+      <c r="B15" s="3">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>53</v>
+      </c>
+      <c r="G15">
+        <v>42</v>
+      </c>
+      <c r="H15">
+        <v>74</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>36</v>
+      </c>
+      <c r="K15">
+        <v>49</v>
+      </c>
+      <c r="L15">
+        <v>0.27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2">
+        <v>37617</v>
+      </c>
+      <c r="B16" s="3">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>44</v>
+      </c>
+      <c r="G16">
+        <v>39</v>
+      </c>
+      <c r="H16">
+        <v>85</v>
+      </c>
+      <c r="I16">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <v>32</v>
+      </c>
+      <c r="K16">
+        <v>48</v>
+      </c>
+      <c r="L16">
+        <v>0.19</v>
+      </c>
+      <c r="M16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2">
+        <v>39817</v>
+      </c>
+      <c r="B17" s="3">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>29</v>
+      </c>
+      <c r="H17">
+        <v>84</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>17</v>
+      </c>
+      <c r="K17">
+        <v>25</v>
+      </c>
+      <c r="L17">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2">
+        <v>41650</v>
+      </c>
+      <c r="B18" s="3">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>52</v>
+      </c>
+      <c r="G18">
+        <v>42</v>
+      </c>
+      <c r="H18">
+        <v>74</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>41</v>
+      </c>
+      <c r="K18">
+        <v>56</v>
+      </c>
+      <c r="L18">
+        <v>0.84</v>
+      </c>
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2">
+        <v>41972</v>
+      </c>
+      <c r="B19" s="3">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>32</v>
+      </c>
+      <c r="G19">
+        <v>24</v>
+      </c>
+      <c r="H19">
+        <v>71</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19">
+        <v>31</v>
+      </c>
+      <c r="K19">
+        <v>39</v>
+      </c>
+      <c r="L19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2">
+        <v>39064</v>
+      </c>
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>47</v>
+      </c>
+      <c r="G20">
+        <v>41</v>
+      </c>
+      <c r="H20">
+        <v>86</v>
+      </c>
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>39</v>
+      </c>
+      <c r="K20">
+        <v>47</v>
+      </c>
+      <c r="L20">
+        <v>0.26</v>
+      </c>
+      <c r="M20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2">
+        <v>40526</v>
+      </c>
+      <c r="B21" s="3">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>43</v>
+      </c>
+      <c r="G21">
+        <v>38</v>
+      </c>
+      <c r="H21">
+        <v>84</v>
+      </c>
+      <c r="I21">
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>36</v>
+      </c>
+      <c r="K21">
+        <v>51</v>
+      </c>
+      <c r="L21">
+        <v>0.82</v>
+      </c>
+      <c r="M21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="2">
+        <v>42439</v>
+      </c>
+      <c r="B22" s="3">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>49</v>
+      </c>
+      <c r="G22">
+        <v>42</v>
+      </c>
+      <c r="H22">
+        <v>75</v>
+      </c>
+      <c r="I22">
+        <v>16</v>
+      </c>
+      <c r="J22">
+        <v>35</v>
+      </c>
+      <c r="K22">
+        <v>45</v>
+      </c>
+      <c r="L22">
+        <v>0.23</v>
+      </c>
+      <c r="M22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="2">
+        <v>37176</v>
+      </c>
+      <c r="B23" s="3">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>52</v>
+      </c>
+      <c r="G23">
+        <v>47</v>
+      </c>
+      <c r="H23">
+        <v>85</v>
+      </c>
+      <c r="I23">
+        <v>14</v>
+      </c>
+      <c r="J23">
+        <v>29</v>
+      </c>
+      <c r="K23">
+        <v>34</v>
+      </c>
+      <c r="L23">
+        <v>0.04</v>
+      </c>
+      <c r="M23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="2">
+        <v>40497</v>
+      </c>
+      <c r="B24" s="3">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>52</v>
+      </c>
+      <c r="G24">
+        <v>49</v>
+      </c>
+      <c r="H24">
+        <v>82</v>
+      </c>
+      <c r="I24">
+        <v>15</v>
+      </c>
+      <c r="J24">
+        <v>36</v>
+      </c>
+      <c r="K24">
+        <v>49</v>
+      </c>
+      <c r="L24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(D1:D24)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:L26" si="0">AVERAGE(E1:E24)</f>
+        <v>0.875</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>47.666666666666664</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>40.75</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>77.875</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>14.75</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>35.375</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>48.956521739130437</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>0.47250000000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2">
+        <v>41103</v>
+      </c>
+      <c r="B1" s="3">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="F1">
+        <v>66</v>
+      </c>
+      <c r="G1">
+        <v>55</v>
+      </c>
+      <c r="H1">
+        <v>70</v>
+      </c>
+      <c r="I1">
+        <v>5</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>17</v>
+      </c>
+      <c r="L1">
+        <v>0.02</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2">
+        <v>42094</v>
+      </c>
+      <c r="B2" s="3">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>49</v>
+      </c>
+      <c r="G2">
+        <v>41</v>
+      </c>
+      <c r="H2">
+        <v>67</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>0.04</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2">
+        <v>41532</v>
+      </c>
+      <c r="B3" s="3">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>62</v>
+      </c>
+      <c r="G3">
+        <v>58</v>
+      </c>
+      <c r="H3">
+        <v>86</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>0.13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2">
+        <v>41853</v>
+      </c>
+      <c r="B4" s="3">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>73</v>
+      </c>
+      <c r="G4">
+        <v>57</v>
+      </c>
+      <c r="H4">
+        <v>61</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>0.02</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2">
+        <v>42230</v>
+      </c>
+      <c r="B5" s="3">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>57</v>
+      </c>
+      <c r="H5">
+        <v>83</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+      <c r="J5">
+        <v>21</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>1.2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2">
+        <v>41522</v>
+      </c>
+      <c r="B6" s="3">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>64</v>
+      </c>
+      <c r="G6">
+        <v>58</v>
+      </c>
+      <c r="H6">
+        <v>83</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>14</v>
+      </c>
+      <c r="K6">
+        <v>17</v>
+      </c>
+      <c r="L6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2">
+        <v>42228</v>
+      </c>
+      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>73</v>
+      </c>
+      <c r="G7">
+        <v>56</v>
+      </c>
+      <c r="H7">
+        <v>59</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>17</v>
+      </c>
+      <c r="K7">
+        <v>22</v>
+      </c>
+      <c r="L7">
+        <v>0.3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <f>AVERAGE(D1:D7)</f>
+        <v>1.8571428571428572</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:L9" si="0">AVERAGE(E1:E7)</f>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>64.142857142857139</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>54.571428571428569</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>72.714285714285708</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>6.7142857142857144</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>22.666666666666668</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>